<commit_message>
Fixes default energy assets, energy flows
-Default energy assets are updated
-energy flow returns restored to operate-function to force return values
</commit_message>
<xml_diff>
--- a/Base/db_defaultEnergyAssets.xlsx
+++ b/Base/db_defaultEnergyAssets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DFA086-2D17-441A-BDDB-B616D8B5E926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5738A1A4-D004-4229-B327-71C9CF7EB1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
   </bookViews>
   <sheets>
     <sheet name="consumptionAssets" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
First basic heating system operational
</commit_message>
<xml_diff>
--- a/Base/db_defaultEnergyAssets.xlsx
+++ b/Base/db_defaultEnergyAssets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBA8F46-BD74-4FC0-854B-A95539C156F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EFE5621-7814-4C9B-A8EB-A7DF331F23A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
+    <workbookView xWindow="3456" yWindow="3456" windowWidth="23040" windowHeight="12156" activeTab="3" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
   </bookViews>
   <sheets>
     <sheet name="consumptionAssets" sheetId="1" r:id="rId1"/>
@@ -592,19 +592,19 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.625" customWidth="1"/>
     <col min="3" max="3" width="36.5" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="42.33203125" customWidth="1"/>
+    <col min="5" max="5" width="42.375" customWidth="1"/>
     <col min="6" max="6" width="24.5" customWidth="1"/>
-    <col min="7" max="7" width="16.83203125" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
-    <col min="11" max="11" width="17.1640625" customWidth="1"/>
+    <col min="7" max="7" width="16.875" customWidth="1"/>
+    <col min="10" max="10" width="13.625" customWidth="1"/>
+    <col min="11" max="11" width="17.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -627,7 +627,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -650,7 +650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -673,7 +673,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -696,7 +696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -732,15 +732,15 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="37.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" customWidth="1"/>
+    <col min="2" max="3" width="37.625" customWidth="1"/>
+    <col min="4" max="4" width="22.875" customWidth="1"/>
     <col min="5" max="5" width="19.5" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+    <col min="6" max="6" width="23.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -763,7 +763,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -787,7 +787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -811,7 +811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -835,7 +835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -859,7 +859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -882,7 +882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -905,7 +905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -941,15 +941,15 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.83203125" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" customWidth="1"/>
-    <col min="4" max="5" width="21.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="23.875" customWidth="1"/>
+    <col min="3" max="3" width="24.125" customWidth="1"/>
+    <col min="4" max="5" width="21.625" customWidth="1"/>
+    <col min="6" max="6" width="17.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -972,7 +972,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -995,7 +995,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1119,22 +1119,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AD685B-9C82-478E-8117-8BE8411F8B92}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.375" customWidth="1"/>
+    <col min="4" max="4" width="20.375" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" customWidth="1"/>
-    <col min="8" max="12" width="21.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.875" customWidth="1"/>
+    <col min="8" max="12" width="21.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1240,16 +1240,16 @@
         <v>50</v>
       </c>
       <c r="J3">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1278,16 +1278,16 @@
         <v>50</v>
       </c>
       <c r="J4">
-        <v>0.6</v>
+        <v>60</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1316,16 +1316,16 @@
         <v>50</v>
       </c>
       <c r="J5">
-        <v>0.7</v>
+        <v>70</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1354,16 +1354,16 @@
         <v>50</v>
       </c>
       <c r="J6">
-        <v>0.8</v>
+        <v>80</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1392,16 +1392,16 @@
         <v>50</v>
       </c>
       <c r="J7">
-        <v>0.9</v>
+        <v>90</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1430,16 +1430,16 @@
         <v>50</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1468,16 +1468,16 @@
         <v>50</v>
       </c>
       <c r="J9">
-        <v>1.1000000000000001</v>
+        <v>110</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="G11">
         <v>0.5</v>
@@ -1544,13 +1544,13 @@
         <v>90</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
-        <v>10000</v>
+        <v>100000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Temperature controller for DH thermal storage
</commit_message>
<xml_diff>
--- a/Base/db_defaultEnergyAssets.xlsx
+++ b/Base/db_defaultEnergyAssets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211666E4-597F-4842-AD84-8DC7FF118E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06506D1D-006C-4EAD-9BD1-8D82F6062704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
+    <workbookView xWindow="-30096" yWindow="624" windowWidth="23040" windowHeight="12156" activeTab="2" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
   </bookViews>
   <sheets>
     <sheet name="consumptionAssets" sheetId="1" r:id="rId1"/>
@@ -948,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE703926-9782-410D-9F5D-95B93C05724F}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1138,7 +1138,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="G8">
         <v>0.95</v>
@@ -1153,8 +1153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AD685B-9C82-478E-8117-8BE8411F8B92}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1261,8 +1261,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="2">
-        <f>20*100/1000</f>
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="G3">
         <v>0.5</v>
@@ -1300,8 +1299,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="2">
-        <f>30*100/1000</f>
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="G4">
         <v>0.5</v>
@@ -1339,8 +1337,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="2">
-        <f>40*100/1000</f>
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="G5">
         <v>0.5</v>
@@ -1378,8 +1375,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="2">
-        <f>40*125/1000</f>
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="G6">
         <v>0.5</v>
@@ -1417,8 +1413,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="2">
-        <f>40*150/1000</f>
-        <v>6</v>
+        <v>100</v>
       </c>
       <c r="G7">
         <v>0.5</v>
@@ -1456,8 +1451,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="2">
-        <f>60*125/1000</f>
-        <v>7.5</v>
+        <v>100</v>
       </c>
       <c r="G8">
         <v>0.5</v>
@@ -1495,8 +1489,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="2">
-        <f>60*150/1000</f>
-        <v>9</v>
+        <v>100</v>
       </c>
       <c r="G9">
         <v>0.5</v>
@@ -1572,7 +1565,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="G11">
         <v>0.5</v>

</xml_diff>

<commit_message>
Added selfConsumption and selfSufficiency calculations for NetConnection agents
*Only works properly is Storage-assets are 'balanced' over the simulation!
</commit_message>
<xml_diff>
--- a/Base/db_defaultEnergyAssets.xlsx
+++ b/Base/db_defaultEnergyAssets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06506D1D-006C-4EAD-9BD1-8D82F6062704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74500A61-4A91-4A71-B5D2-EF89AAEE0689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30096" yWindow="624" windowWidth="23040" windowHeight="12156" activeTab="2" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="3" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
   </bookViews>
   <sheets>
     <sheet name="consumptionAssets" sheetId="1" r:id="rId1"/>
@@ -948,7 +948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE703926-9782-410D-9F5D-95B93C05724F}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -1153,8 +1153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AD685B-9C82-478E-8117-8BE8411F8B92}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1530,7 +1530,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H10">
         <v>0</v>

</xml_diff>

<commit_message>
Consumption assets profiles scaled by yearly demand, data-agnostic heat network
** Consumption type energy assets schalen bepalen nu hun vermogensvraag a.d.h.v. hun jaarlijkse vraag in MWh en genormaliseerd vraagprofiel (telt op tot 1).
** werkende profiles toegevoegd voor house_electricity_demand_other en building_electricity_demand_other, house_heat_demand_hot_water.
** Technical debt: gehardcode energyAssets voor districtHeating data-agnost gemaakt via defaultEnergyAssets
</commit_message>
<xml_diff>
--- a/Base/db_defaultEnergyAssets.xlsx
+++ b/Base/db_defaultEnergyAssets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\Base\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2E5947-CBD6-4B7F-B2DE-3E1D1F702B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3906FF44-1BEF-4286-B60E-3E8CE4E658E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7125" yWindow="2055" windowWidth="38700" windowHeight="15375" activeTab="3" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
   </bookViews>
   <sheets>
     <sheet name="consumptionAssets" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="73">
   <si>
     <t>id</t>
   </si>
@@ -242,6 +242,21 @@
   </si>
   <si>
     <t>HEAT_DELIVERY_SET</t>
+  </si>
+  <si>
+    <t>yearlyDemandElectricity_kWh</t>
+  </si>
+  <si>
+    <t>yearlyDemandHeat_kWh</t>
+  </si>
+  <si>
+    <t>setTemp_degC</t>
+  </si>
+  <si>
+    <t>District_Heating_network_HT_S</t>
+  </si>
+  <si>
+    <t>District_Heating_network_MT_S</t>
   </si>
 </sst>
 </file>
@@ -279,10 +294,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,7 +616,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -609,8 +625,8 @@
     <col min="3" max="3" width="36.5" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="42.33203125" customWidth="1"/>
-    <col min="6" max="6" width="24.5" customWidth="1"/>
-    <col min="7" max="7" width="16.83203125" customWidth="1"/>
+    <col min="6" max="6" width="27.5" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" customWidth="1"/>
     <col min="11" max="11" width="17.1640625" customWidth="1"/>
   </cols>
@@ -632,10 +648,10 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -655,7 +671,7 @@
         <v>23</v>
       </c>
       <c r="F2">
-        <v>11</v>
+        <v>2479</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -701,7 +717,8 @@
         <v>23</v>
       </c>
       <c r="F4">
-        <v>30</v>
+        <f>60*2000</f>
+        <v>120000</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -724,7 +741,8 @@
         <v>23</v>
       </c>
       <c r="F5">
-        <v>20</v>
+        <f>35*1000</f>
+        <v>35000</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -1151,10 +1169,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AD685B-9C82-478E-8117-8BE8411F8B92}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1165,10 +1183,10 @@
     <col min="5" max="5" width="21" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="15.83203125" customWidth="1"/>
-    <col min="8" max="12" width="21.33203125" customWidth="1"/>
+    <col min="8" max="13" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1197,16 +1215,19 @@
         <v>14</v>
       </c>
       <c r="J1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>21</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1238,13 +1259,16 @@
         <v>0</v>
       </c>
       <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
         <v>50</v>
       </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1273,16 +1297,19 @@
         <v>50</v>
       </c>
       <c r="J3">
+        <v>20</v>
+      </c>
+      <c r="K3">
         <v>50</v>
       </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
       <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
         <v>10000000</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1311,16 +1338,19 @@
         <v>50</v>
       </c>
       <c r="J4">
+        <v>20</v>
+      </c>
+      <c r="K4">
         <v>60</v>
       </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
       <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
         <v>10000000</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1349,16 +1379,19 @@
         <v>50</v>
       </c>
       <c r="J5">
+        <v>20</v>
+      </c>
+      <c r="K5">
         <v>70</v>
       </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5" s="1">
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
         <v>10000000</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1387,16 +1420,19 @@
         <v>50</v>
       </c>
       <c r="J6">
+        <v>20</v>
+      </c>
+      <c r="K6">
         <v>80</v>
       </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6" s="1">
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
         <v>10000000</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1425,16 +1461,19 @@
         <v>50</v>
       </c>
       <c r="J7">
+        <v>20</v>
+      </c>
+      <c r="K7">
         <v>90</v>
       </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7" s="1">
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
         <v>10000000</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1463,16 +1502,19 @@
         <v>50</v>
       </c>
       <c r="J8">
+        <v>20</v>
+      </c>
+      <c r="K8">
         <v>100</v>
       </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8" s="1">
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
         <v>10000000</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1501,16 +1543,19 @@
         <v>50</v>
       </c>
       <c r="J9">
+        <v>20</v>
+      </c>
+      <c r="K9">
         <v>110</v>
       </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9" s="1">
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
         <v>10000000</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1542,13 +1587,16 @@
         <v>0</v>
       </c>
       <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
         <v>50</v>
       </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1568,22 +1616,108 @@
         <v>1000</v>
       </c>
       <c r="G11">
-        <v>0.66659999999999997</v>
+        <f>0.2</f>
+        <v>0.2</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="I11">
         <v>90</v>
       </c>
       <c r="J11">
+        <v>60</v>
+      </c>
+      <c r="K11">
         <v>1000</v>
       </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11" s="1">
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
         <v>100000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1000</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>70</v>
+      </c>
+      <c r="I12">
+        <v>100</v>
+      </c>
+      <c r="J12">
+        <v>90</v>
+      </c>
+      <c r="K12">
+        <v>100</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1000</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>60</v>
+      </c>
+      <c r="I13">
+        <v>80</v>
+      </c>
+      <c r="J13">
+        <v>70</v>
+      </c>
+      <c r="K13">
+        <v>100</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <v>10000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Heat network assets data-agnostisch, fixes
**District heating verder data-agnostisch gemaakt m.b.v. default energy assets. Parameter tweaks. Warmtepomp+gas-peak variant toegevoegd.
Bug: warmteverlies in district heating network gaat nog iets mis
**Kleine tweaks in configdata voor gridConnections en tweede heat-node
**kleine fixes hernoemen variabelen naar (grid ipv net)
</commit_message>
<xml_diff>
--- a/Base/db_defaultEnergyAssets.xlsx
+++ b/Base/db_defaultEnergyAssets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3906FF44-1BEF-4286-B60E-3E8CE4E658E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5FFACA-B1A1-462E-8907-AC74E94702AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="76">
   <si>
     <t>id</t>
   </si>
@@ -148,15 +148,6 @@
     <t>Windmill_7MW</t>
   </si>
   <si>
-    <t>House_heatpump_S</t>
-  </si>
-  <si>
-    <t>House_heatpump_M</t>
-  </si>
-  <si>
-    <t>House_heatpump_L</t>
-  </si>
-  <si>
     <t>Solarpanels_1MW</t>
   </si>
   <si>
@@ -235,9 +226,6 @@
     <t>House_heatmodel_G</t>
   </si>
   <si>
-    <t>District_Heating_heat_buffer_S</t>
-  </si>
-  <si>
     <t>House_DH_heatdeliveryset</t>
   </si>
   <si>
@@ -257,6 +245,27 @@
   </si>
   <si>
     <t>District_Heating_network_MT_S</t>
+  </si>
+  <si>
+    <t>District_Heating_heat_buffer_HT_S</t>
+  </si>
+  <si>
+    <t>HEAT_PUMP_GROUND</t>
+  </si>
+  <si>
+    <t>House_heatpump_MT_S</t>
+  </si>
+  <si>
+    <t>House_heatpump_MT_M</t>
+  </si>
+  <si>
+    <t>House_heatpump_MT_L</t>
+  </si>
+  <si>
+    <t>DH_heat_pump_HT_S</t>
+  </si>
+  <si>
+    <t>deliveryTemp_degc</t>
   </si>
 </sst>
 </file>
@@ -648,10 +657,10 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -659,10 +668,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -682,10 +691,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -705,10 +714,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -729,10 +738,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -800,7 +809,7 @@
         <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -824,7 +833,7 @@
         <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -848,7 +857,7 @@
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
@@ -872,7 +881,7 @@
         <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
@@ -896,7 +905,7 @@
         <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -919,7 +928,7 @@
         <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
@@ -939,10 +948,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
@@ -964,10 +973,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE703926-9782-410D-9F5D-95B93C05724F}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -978,7 +987,7 @@
     <col min="6" max="6" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1000,13 +1009,16 @@
       <c r="G1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -1023,13 +1035,16 @@
       <c r="G2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -1046,13 +1061,16 @@
       <c r="G3">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -1069,13 +1087,16 @@
       <c r="G4">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1092,19 +1113,22 @@
       <c r="G5">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1115,8 +1139,11 @@
       <c r="G6">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1138,13 +1165,16 @@
       <c r="G7">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -1160,6 +1190,35 @@
       </c>
       <c r="G8">
         <v>0.95</v>
+      </c>
+      <c r="H8">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0.5</v>
+      </c>
+      <c r="H9">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1172,12 +1231,12 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" customWidth="1"/>
     <col min="3" max="3" width="21.33203125" customWidth="1"/>
     <col min="4" max="4" width="20.33203125" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
@@ -1215,7 +1274,7 @@
         <v>14</v>
       </c>
       <c r="J1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K1" t="s">
         <v>12</v>
@@ -1232,7 +1291,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1273,7 +1332,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -1314,7 +1373,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -1355,7 +1414,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -1396,7 +1455,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1437,7 +1496,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -1478,7 +1537,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -1519,7 +1578,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -1601,7 +1660,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -1616,17 +1675,16 @@
         <v>1000</v>
       </c>
       <c r="G11">
-        <f>0.2</f>
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="I11">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="J11">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="K11">
         <v>1000</v>
@@ -1643,7 +1701,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -1684,7 +1742,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Data agnostic heatingSystemTypes, isolationLabels, fixes
* Het type heatingsysteem voor gridConnections wordt nu extern meegegeven in de backboneConfigExcel en json.
* Het schillabel van houses en buildings wordt nu extern meegegeven in de backBoneConfigExcel en json.
* Houses hebben nu een werkend energielabel en bijbehorend warmtevraagmodel
* Heat Storage en -Conversion energyassets die afhankelijk zijn van buitentemperatuur worden nu uurlijks voorzien van de juiste waarden hiervoor, vanuit main. Bodemtemperatuur-afhankelijke assets krijgen deze temperatuur éénmalig mee bij opstart.
* Fix: heat conversion- en storageAssets werden nog niet ge-operate in de nieuwe structuur. Dit werkt nu weer.
* Lege GCIndustry agenttype en population aangemaakt
* Profielen voor industry_steel en industry_other uit ETM in profiles-excel toegevoegd
* Run starttijd teruggezet naar 1-1-2022 zodat tijdreeksdata klopt bij de datum.
</commit_message>
<xml_diff>
--- a/Base/db_defaultEnergyAssets.xlsx
+++ b/Base/db_defaultEnergyAssets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5FFACA-B1A1-462E-8907-AC74E94702AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140D52FC-A88A-4509-882B-2C135E61F9C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
   </bookViews>
   <sheets>
     <sheet name="consumptionAssets" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="79">
   <si>
     <t>id</t>
   </si>
@@ -266,6 +266,15 @@
   </si>
   <si>
     <t>deliveryTemp_degc</t>
+  </si>
+  <si>
+    <t>AIR</t>
+  </si>
+  <si>
+    <t>GROUND</t>
+  </si>
+  <si>
+    <t>ambientTempType</t>
   </si>
 </sst>
 </file>
@@ -973,10 +982,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE703926-9782-410D-9F5D-95B93C05724F}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -987,7 +996,7 @@
     <col min="6" max="6" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1012,8 +1021,11 @@
       <c r="H1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1038,8 +1050,11 @@
       <c r="H2">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1064,8 +1079,11 @@
       <c r="H3">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1090,8 +1108,11 @@
       <c r="H4">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1117,7 +1138,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1142,8 +1163,11 @@
       <c r="H6">
         <v>90</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1169,7 +1193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1195,7 +1219,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1209,7 +1233,7 @@
         <v>70</v>
       </c>
       <c r="E9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1219,6 +1243,9 @@
       </c>
       <c r="H9">
         <v>90</v>
+      </c>
+      <c r="I9" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1228,10 +1255,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AD685B-9C82-478E-8117-8BE8411F8B92}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1243,9 +1270,10 @@
     <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="15.83203125" customWidth="1"/>
     <col min="8" max="13" width="21.33203125" customWidth="1"/>
+    <col min="14" max="14" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1285,8 +1313,11 @@
       <c r="M1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1327,7 +1358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1367,8 +1398,11 @@
       <c r="M3">
         <v>10000000</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1408,8 +1442,11 @@
       <c r="M4">
         <v>10000000</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1449,8 +1486,11 @@
       <c r="M5" s="1">
         <v>10000000</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1490,8 +1530,11 @@
       <c r="M6" s="1">
         <v>10000000</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1531,8 +1574,11 @@
       <c r="M7" s="1">
         <v>10000000</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1572,8 +1618,11 @@
       <c r="M8" s="1">
         <v>10000000</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1613,8 +1662,11 @@
       <c r="M9" s="1">
         <v>10000000</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1655,7 +1707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1695,8 +1747,11 @@
       <c r="M11" s="1">
         <v>100000000</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1736,8 +1791,11 @@
       <c r="M12" s="1">
         <v>10000000</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1776,6 +1834,9 @@
       </c>
       <c r="M13" s="1">
         <v>10000000</v>
+      </c>
+      <c r="N13" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Overall molecular energy imports and exports, industry case, KPI-Visuals agent fixed
*Totale import en export van methaan en waterstof in het model worden berekend en uitgestuurd als onderdeel van de TotalCostKPI-data aan het einde van de modelrun
*Modelconfiguratie gemaakt voor industrie-case.
*Electric Heavy Goods vehicle toegevoegd in defaultEnergyAssets.xslx
*KPI-Visuals-agent werkt weer, industry-gridconnection-categorie toegevoegd.
</commit_message>
<xml_diff>
--- a/Base/db_defaultEnergyAssets.xlsx
+++ b/Base/db_defaultEnergyAssets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\Base\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44235BE-D609-427A-A1CF-1B1B72164095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFD13EE-484F-4073-890A-6DF521697A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18720" yWindow="4065" windowWidth="28470" windowHeight="16920" activeTab="2" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
   </bookViews>
   <sheets>
     <sheet name="consumptionAssets" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="97">
   <si>
     <t>id</t>
   </si>
@@ -323,6 +323,12 @@
   </si>
   <si>
     <t>BOILER</t>
+  </si>
+  <si>
+    <t>EHGV</t>
+  </si>
+  <si>
+    <t>ELECTRIC_HEAVY_GOODS_VEHICLE</t>
   </si>
 </sst>
 </file>
@@ -681,12 +687,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382AAFBF-1CF8-487E-AF78-99304C1FCDA1}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" customWidth="1"/>
     <col min="3" max="3" width="36.5" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
@@ -915,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E4F107-16BA-4AA1-967F-7283CFA19530}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1124,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE703926-9782-410D-9F5D-95B93C05724F}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1473,10 +1480,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AD685B-9C82-478E-8117-8BE8411F8B92}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2057,6 +2064,47 @@
         <v>77</v>
       </c>
     </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14">
+        <v>110</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>500</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
EV's as electric storage, opgenomen in battery KPIs
*EV's as electric storage
*EV's opgenomen in battery total Cost KPIs
*Aantal units per type toegevoegd aan Battery total cost KPI's
</commit_message>
<xml_diff>
--- a/Base/db_defaultEnergyAssets.xlsx
+++ b/Base/db_defaultEnergyAssets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C82F3AD-DAB0-4CBA-9356-09D50A1C6ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072DAA78-0F3D-49A6-B104-E61E218A1D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
   </bookViews>
   <sheets>
     <sheet name="consumptionAssets" sheetId="1" r:id="rId1"/>
@@ -103,9 +103,6 @@
     <t>ELECTRIC_VEHICLE</t>
   </si>
   <si>
-    <t>chargeCapacity_kWh</t>
-  </si>
-  <si>
     <t>alias</t>
   </si>
   <si>
@@ -332,6 +329,9 @@
   </si>
   <si>
     <t>Grid_battery</t>
+  </si>
+  <si>
+    <t>storageCapacity_kWh</t>
   </si>
 </sst>
 </file>
@@ -715,7 +715,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -724,10 +724,10 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
         <v>64</v>
-      </c>
-      <c r="G1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -735,16 +735,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2">
         <v>2479</v>
@@ -758,16 +758,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -781,16 +781,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4">
         <f>60*2000</f>
@@ -805,16 +805,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5">
         <f>35*1000</f>
@@ -829,16 +829,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F6">
         <v>1000000</v>
@@ -852,16 +852,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -875,16 +875,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F8">
         <v>1000000</v>
@@ -898,16 +898,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -926,7 +926,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -945,7 +945,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -965,10 +965,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -989,10 +989,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -1013,10 +1013,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
@@ -1037,16 +1037,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5">
         <f>3000</f>
@@ -1061,16 +1061,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6">
         <v>5000</v>
@@ -1084,16 +1084,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7">
         <v>7000</v>
@@ -1107,10 +1107,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
@@ -1169,10 +1169,10 @@
         <v>18</v>
       </c>
       <c r="H1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1180,13 +1180,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2">
         <v>4</v>
@@ -1201,7 +1201,7 @@
         <v>60</v>
       </c>
       <c r="I2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1209,13 +1209,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3">
         <v>6</v>
@@ -1230,7 +1230,7 @@
         <v>60</v>
       </c>
       <c r="I3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1238,13 +1238,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4">
         <v>11</v>
@@ -1259,7 +1259,7 @@
         <v>60</v>
       </c>
       <c r="I4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1267,13 +1267,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1293,13 +1293,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1314,7 +1314,7 @@
         <v>90</v>
       </c>
       <c r="I6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1348,13 +1348,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1374,13 +1374,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -1395,7 +1395,7 @@
         <v>90</v>
       </c>
       <c r="I9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1403,13 +1403,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E10">
         <v>300</v>
@@ -1429,13 +1429,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1455,13 +1455,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1485,8 +1485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AD685B-9C82-478E-8117-8BE8411F8B92}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1530,19 +1530,19 @@
         <v>14</v>
       </c>
       <c r="J1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K1" t="s">
         <v>12</v>
       </c>
       <c r="L1" t="s">
-        <v>21</v>
+        <v>97</v>
       </c>
       <c r="M1" t="s">
         <v>15</v>
       </c>
       <c r="N1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -1550,13 +1550,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -1591,13 +1591,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1627,7 +1627,7 @@
         <v>10000000</v>
       </c>
       <c r="N3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -1635,13 +1635,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1671,7 +1671,7 @@
         <v>10000000</v>
       </c>
       <c r="N4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -1679,13 +1679,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1715,7 +1715,7 @@
         <v>10000000</v>
       </c>
       <c r="N5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -1723,13 +1723,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1759,7 +1759,7 @@
         <v>10000000</v>
       </c>
       <c r="N6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -1767,13 +1767,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1803,7 +1803,7 @@
         <v>10000000</v>
       </c>
       <c r="N7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -1811,13 +1811,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1847,7 +1847,7 @@
         <v>10000000</v>
       </c>
       <c r="N8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -1855,13 +1855,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1891,7 +1891,7 @@
         <v>10000000</v>
       </c>
       <c r="N9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -1940,13 +1940,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1976,7 +1976,7 @@
         <v>10000000000</v>
       </c>
       <c r="N11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -1984,13 +1984,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -2020,7 +2020,7 @@
         <v>10000000</v>
       </c>
       <c r="N12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -2028,13 +2028,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -2064,7 +2064,7 @@
         <v>10000000</v>
       </c>
       <c r="N13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -2072,13 +2072,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14">
         <v>1000</v>
@@ -2113,13 +2113,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E15">
         <v>110</v>

</xml_diff>

<commit_message>
Added logistics fleet as pure consumption asset, integrated evaluation in Building gridConnection
</commit_message>
<xml_diff>
--- a/Base/db_defaultEnergyAssets.xlsx
+++ b/Base/db_defaultEnergyAssets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072DAA78-0F3D-49A6-B104-E61E218A1D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F6E699-DF82-452D-9693-7BD20A93A0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
+    <workbookView xWindow="2652" yWindow="2652" windowWidth="26376" windowHeight="12264" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
   </bookViews>
   <sheets>
     <sheet name="consumptionAssets" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="100">
   <si>
     <t>id</t>
   </si>
@@ -328,10 +328,16 @@
     <t>ELECTRIC_HEAVY_GOODS_VEHICLE</t>
   </si>
   <si>
-    <t>Grid_battery</t>
-  </si>
-  <si>
     <t>storageCapacity_kWh</t>
+  </si>
+  <si>
+    <t>Logistics_fleet_hgv_E</t>
+  </si>
+  <si>
+    <t>logistics_fleet_e_hgv</t>
+  </si>
+  <si>
+    <t>Grid_battery_1MWh</t>
   </si>
 </sst>
 </file>
@@ -688,26 +694,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382AAFBF-1CF8-487E-AF78-99304C1FCDA1}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.625" customWidth="1"/>
     <col min="3" max="3" width="36.5" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="42.33203125" customWidth="1"/>
+    <col min="5" max="5" width="42.375" customWidth="1"/>
     <col min="6" max="6" width="27.5" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
-    <col min="11" max="11" width="17.1640625" customWidth="1"/>
+    <col min="7" max="7" width="22.625" customWidth="1"/>
+    <col min="10" max="10" width="13.625" customWidth="1"/>
+    <col min="11" max="11" width="17.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -730,7 +736,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -753,7 +759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -776,7 +782,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -800,7 +806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -824,7 +830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -847,7 +853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -870,7 +876,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -893,7 +899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -914,6 +920,30 @@
       </c>
       <c r="G9">
         <v>1000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10">
+        <f>25*100000*3</f>
+        <v>7500000</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -929,15 +959,15 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="37.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" customWidth="1"/>
+    <col min="2" max="3" width="37.625" customWidth="1"/>
+    <col min="4" max="4" width="22.875" customWidth="1"/>
     <col min="5" max="5" width="19.5" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+    <col min="6" max="6" width="23.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -960,7 +990,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -984,7 +1014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1008,7 +1038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1032,7 +1062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1056,7 +1086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1079,7 +1109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1102,7 +1132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1138,15 +1168,15 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="34.1640625" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" customWidth="1"/>
-    <col min="4" max="5" width="21.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="34.125" customWidth="1"/>
+    <col min="3" max="3" width="24.125" customWidth="1"/>
+    <col min="4" max="5" width="21.625" customWidth="1"/>
+    <col min="6" max="6" width="17.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1175,7 +1205,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1204,7 +1234,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1233,7 +1263,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1262,7 +1292,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1288,7 +1318,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1317,7 +1347,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1343,7 +1373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1369,7 +1399,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1398,7 +1428,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1424,7 +1454,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1450,7 +1480,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1485,23 +1515,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AD685B-9C82-478E-8117-8BE8411F8B92}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="34.33203125" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="34.375" customWidth="1"/>
+    <col min="3" max="3" width="21.375" customWidth="1"/>
+    <col min="4" max="4" width="20.375" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" customWidth="1"/>
-    <col min="8" max="13" width="21.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.875" customWidth="1"/>
+    <col min="8" max="13" width="21.375" customWidth="1"/>
     <col min="14" max="14" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1536,7 +1566,7 @@
         <v>12</v>
       </c>
       <c r="L1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M1" t="s">
         <v>15</v>
@@ -1545,7 +1575,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1586,7 +1616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1630,7 +1660,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1674,7 +1704,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1718,7 +1748,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1762,7 +1792,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1806,7 +1836,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1850,7 +1880,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1894,7 +1924,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1935,7 +1965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1979,7 +2009,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2023,7 +2053,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2067,12 +2097,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -2108,7 +2138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Implemented basic controller of GridBattery to keep HOLON-power within grid capacity
GridBattery is now 10MWh (with 2MW peak charge/discharge power), 2MWp PV is installed, and logistics charging power peaks at around 1.8MW during the night.
This grid connection capacity is 1.2MW.
</commit_message>
<xml_diff>
--- a/Base/db_defaultEnergyAssets.xlsx
+++ b/Base/db_defaultEnergyAssets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F6E699-DF82-452D-9693-7BD20A93A0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A203C26C-CF69-41EC-B08F-44C3197FE8F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="2652" windowWidth="26376" windowHeight="12264" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
+    <workbookView xWindow="17385" yWindow="7410" windowWidth="26370" windowHeight="12270" activeTab="3" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
   </bookViews>
   <sheets>
     <sheet name="consumptionAssets" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="101">
   <si>
     <t>id</t>
   </si>
@@ -338,6 +338,9 @@
   </si>
   <si>
     <t>Grid_battery_1MWh</t>
+  </si>
+  <si>
+    <t>Grid_battery_10MWh</t>
   </si>
 </sst>
 </file>
@@ -696,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382AAFBF-1CF8-487E-AF78-99304C1FCDA1}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
@@ -939,8 +942,8 @@
         <v>86</v>
       </c>
       <c r="F10">
-        <f>25*100000*3</f>
-        <v>7500000</v>
+        <f>60*100000*1.3</f>
+        <v>7800000</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1513,10 +1516,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AD685B-9C82-478E-8117-8BE8411F8B92}">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
@@ -2179,6 +2182,47 @@
         <v>0</v>
       </c>
     </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16">
+        <v>2000</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>10000</v>
+      </c>
+      <c r="M16" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
HOLON power stays within grid capacity
*Adjusted some parameters for battery management
*manually set battery charge setpoint for first timestep (to prevent overconsumption on modelstart)
*'froze' consumption of logistics fleet during last hour to prevent sudden step up in power. Actually, all tablefunctions 'loop' back to first hour of year during last hour of the simulation if you don't do this!
</commit_message>
<xml_diff>
--- a/Base/db_defaultEnergyAssets.xlsx
+++ b/Base/db_defaultEnergyAssets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A203C26C-CF69-41EC-B08F-44C3197FE8F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433C119D-B8D6-4A59-B14B-7A8730AF6C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17385" yWindow="7410" windowWidth="26370" windowHeight="12270" activeTab="3" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
+    <workbookView xWindow="2205" yWindow="2490" windowWidth="26370" windowHeight="16995" activeTab="1" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
   </bookViews>
   <sheets>
     <sheet name="consumptionAssets" sheetId="1" r:id="rId1"/>
@@ -700,23 +700,23 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="23.625" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
     <col min="3" max="3" width="36.5" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="42.375" customWidth="1"/>
+    <col min="5" max="5" width="42.33203125" customWidth="1"/>
     <col min="6" max="6" width="27.5" customWidth="1"/>
-    <col min="7" max="7" width="22.625" customWidth="1"/>
-    <col min="10" max="10" width="13.625" customWidth="1"/>
-    <col min="11" max="11" width="17.125" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -739,7 +739,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -762,7 +762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -785,7 +785,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -809,7 +809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -833,7 +833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -856,7 +856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -879,7 +879,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -902,7 +902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -925,7 +925,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -942,8 +942,8 @@
         <v>86</v>
       </c>
       <c r="F10">
-        <f>60*100000*1.3</f>
-        <v>7800000</v>
+        <f>50*100000*1.3</f>
+        <v>6500000</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -958,19 +958,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E4F107-16BA-4AA1-967F-7283CFA19530}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="37.625" customWidth="1"/>
-    <col min="4" max="4" width="22.875" customWidth="1"/>
+    <col min="2" max="3" width="37.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" customWidth="1"/>
     <col min="5" max="5" width="19.5" customWidth="1"/>
-    <col min="6" max="6" width="23.375" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -993,7 +993,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1171,15 +1171,15 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="34.125" customWidth="1"/>
-    <col min="3" max="3" width="24.125" customWidth="1"/>
-    <col min="4" max="5" width="21.625" customWidth="1"/>
-    <col min="6" max="6" width="17.125" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" customWidth="1"/>
+    <col min="4" max="5" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1518,23 +1518,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AD685B-9C82-478E-8117-8BE8411F8B92}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="34.375" customWidth="1"/>
-    <col min="3" max="3" width="21.375" customWidth="1"/>
-    <col min="4" max="4" width="20.375" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="15.875" customWidth="1"/>
-    <col min="8" max="13" width="21.375" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="8" max="13" width="21.33203125" customWidth="1"/>
     <col min="14" max="14" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Data input for trucks
E-trucks input data agnost gemaakt
</commit_message>
<xml_diff>
--- a/Base/db_defaultEnergyAssets.xlsx
+++ b/Base/db_defaultEnergyAssets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/p_hogeveen_tue_nl/Documents/HOLON/Base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{00F6E699-DF82-452D-9693-7BD20A93A0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EE8ADF1-3104-40FC-A8C1-05D521456E4B}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{00F6E699-DF82-452D-9693-7BD20A93A0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F941BF79-112F-4279-9746-31C22607645F}"/>
   <bookViews>
     <workbookView xWindow="1125" yWindow="795" windowWidth="24450" windowHeight="11385" activeTab="3" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="100">
   <si>
     <t>id</t>
   </si>
@@ -334,6 +334,9 @@
   </si>
   <si>
     <t>Grid_battery_1MWh</t>
+  </si>
+  <si>
+    <t>energy_consumption_kwhpkm</t>
   </si>
 </sst>
 </file>
@@ -1509,10 +1512,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AD685B-9C82-478E-8117-8BE8411F8B92}">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1527,7 +1530,7 @@
     <col min="14" max="14" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1570,8 +1573,11 @@
       <c r="N1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1611,8 +1617,11 @@
       <c r="M2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1655,8 +1664,11 @@
       <c r="N3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1699,8 +1711,11 @@
       <c r="N4" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1743,8 +1758,11 @@
       <c r="N5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1787,8 +1805,11 @@
       <c r="N6" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1831,8 +1852,11 @@
       <c r="N7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1875,8 +1899,11 @@
       <c r="N8" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1919,8 +1946,11 @@
       <c r="N9" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1960,8 +1990,11 @@
       <c r="M10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2004,8 +2037,11 @@
       <c r="N11" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2048,8 +2084,11 @@
       <c r="N12" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2092,8 +2131,11 @@
       <c r="N13" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2133,8 +2175,11 @@
       <c r="M14" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2173,6 +2218,9 @@
       </c>
       <c r="M15">
         <v>0</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-added 10MWh GridBattery in defaultAssets excel after merge
</commit_message>
<xml_diff>
--- a/Base/db_defaultEnergyAssets.xlsx
+++ b/Base/db_defaultEnergyAssets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/p_hogeveen_tue_nl/Documents/HOLON/Base/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{00F6E699-DF82-452D-9693-7BD20A93A0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F941BF79-112F-4279-9746-31C22607645F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B835AED-BA96-4D67-9010-FD1BBFAD0A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="795" windowWidth="24450" windowHeight="11385" activeTab="3" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
   </bookViews>
   <sheets>
     <sheet name="consumptionAssets" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="101">
   <si>
     <t>id</t>
   </si>
@@ -337,6 +337,9 @@
   </si>
   <si>
     <t>energy_consumption_kwhpkm</t>
+  </si>
+  <si>
+    <t>Grid_battery_10MWh</t>
   </si>
 </sst>
 </file>
@@ -1512,10 +1515,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AD685B-9C82-478E-8117-8BE8411F8B92}">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2155,7 +2158,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -2221,6 +2224,50 @@
       </c>
       <c r="O15">
         <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16">
+        <v>2000</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0.8</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>10000</v>
+      </c>
+      <c r="M16" s="1">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes to EV charging behavior (preventing charging peaks of 3+MW)
Model now supports multiple vehicles per gridConnection, but only in the 'Industry' grid-connection. (Should be moved to the parent GridConnection agent I think)
</commit_message>
<xml_diff>
--- a/Base/db_defaultEnergyAssets.xlsx
+++ b/Base/db_defaultEnergyAssets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B835AED-BA96-4D67-9010-FD1BBFAD0A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019DF3B8-FEF1-48BF-BC16-77DCE83EC9BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
   </bookViews>
   <sheets>
     <sheet name="consumptionAssets" sheetId="1" r:id="rId1"/>
@@ -698,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382AAFBF-1CF8-487E-AF78-99304C1FCDA1}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -941,8 +941,8 @@
         <v>86</v>
       </c>
       <c r="F10">
-        <f>25*100000*3</f>
-        <v>7500000</v>
+        <f>50*100000*1.3</f>
+        <v>6500000</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1517,8 +1517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AD685B-9C82-478E-8117-8BE8411F8B92}">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2196,7 +2196,7 @@
         <v>20</v>
       </c>
       <c r="E15">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="F15">
         <v>0</v>

</xml_diff>

<commit_message>
Preprocessing module scripts from other branch
Preprocessing module scripts from the other explicitEnergyAssets branch
</commit_message>
<xml_diff>
--- a/Base/db_defaultEnergyAssets.xlsx
+++ b/Base/db_defaultEnergyAssets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\Base\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019DF3B8-FEF1-48BF-BC16-77DCE83EC9BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737D6D19-C2F8-42DE-9A9E-62C0A5AD2A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
   </bookViews>
   <sheets>
     <sheet name="consumptionAssets" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="127">
   <si>
     <t>id</t>
   </si>
@@ -324,6 +325,9 @@
     <t>EHGV</t>
   </si>
   <si>
+    <t>ELECTRIC_HEAVY_GOODS_VEHICLE</t>
+  </si>
+  <si>
     <t>storageCapacity_kWh</t>
   </si>
   <si>
@@ -336,10 +340,85 @@
     <t>Grid_battery_1MWh</t>
   </si>
   <si>
-    <t>energy_consumption_kwhpkm</t>
-  </si>
-  <si>
     <t>Grid_battery_10MWh</t>
+  </si>
+  <si>
+    <t>Building_solarpanels_1kWp</t>
+  </si>
+  <si>
+    <t>Solar panels for building, 1 kWp</t>
+  </si>
+  <si>
+    <t>Building_solarpanels_0kWp</t>
+  </si>
+  <si>
+    <t>Solar panels for building, 0 kWp</t>
+  </si>
+  <si>
+    <t>Building_gas_burner_60kW</t>
+  </si>
+  <si>
+    <t>Solarpanels_0MW</t>
+  </si>
+  <si>
+    <t>Solarpanels_2MW</t>
+  </si>
+  <si>
+    <t>Solarpanels_3MW</t>
+  </si>
+  <si>
+    <t>Building_solarpanels_2kWp</t>
+  </si>
+  <si>
+    <t>Building_solarpanels_3kWp</t>
+  </si>
+  <si>
+    <t>Building_solarpanels_4kWp</t>
+  </si>
+  <si>
+    <t>Building_solarpanels_5kWp</t>
+  </si>
+  <si>
+    <t>Solar panels for building, 2 kWp</t>
+  </si>
+  <si>
+    <t>Solar panels for building, 3 kWp</t>
+  </si>
+  <si>
+    <t>Solar panels for building, 4 kWp</t>
+  </si>
+  <si>
+    <t>Solar panels for building, 5 kWp</t>
+  </si>
+  <si>
+    <t>Solar field 2 MW</t>
+  </si>
+  <si>
+    <t>Solar field 3 MW</t>
+  </si>
+  <si>
+    <t>Solar field 4 MW</t>
+  </si>
+  <si>
+    <t>Solarpanels_4MW</t>
+  </si>
+  <si>
+    <t>Solarpanels_5MW</t>
+  </si>
+  <si>
+    <t>Solarpanels_6MW</t>
+  </si>
+  <si>
+    <t>Solar field 5 MW</t>
+  </si>
+  <si>
+    <t>Solar field 6 MW</t>
+  </si>
+  <si>
+    <t>Solar field 0 MW</t>
+  </si>
+  <si>
+    <t>Building_heatpump_20kW</t>
   </si>
 </sst>
 </file>
@@ -698,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382AAFBF-1CF8-487E-AF78-99304C1FCDA1}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -929,10 +1008,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
@@ -955,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E4F107-16BA-4AA1-967F-7283CFA19530}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1139,10 +1218,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>106</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>125</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
@@ -1151,9 +1230,276 @@
         <v>9</v>
       </c>
       <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9">
         <v>1000</v>
       </c>
-      <c r="G8">
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>2000</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <v>3000</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19">
+        <v>4</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+      <c r="G20">
         <v>0</v>
       </c>
     </row>
@@ -1164,10 +1510,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE703926-9782-410D-9F5D-95B93C05724F}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1508,6 +1854,61 @@
         <v>120</v>
       </c>
     </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>60</v>
+      </c>
+      <c r="G13">
+        <v>0.95</v>
+      </c>
+      <c r="H13">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14">
+        <v>20</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0.6</v>
+      </c>
+      <c r="H14">
+        <v>60</v>
+      </c>
+      <c r="I14" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1515,17 +1916,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AD685B-9C82-478E-8117-8BE8411F8B92}">
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="34.33203125" customWidth="1"/>
     <col min="3" max="3" width="21.33203125" customWidth="1"/>
-    <col min="4" max="4" width="33.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="15.83203125" customWidth="1"/>
@@ -1533,7 +1934,7 @@
     <col min="14" max="14" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1568,7 +1969,7 @@
         <v>12</v>
       </c>
       <c r="L1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M1" t="s">
         <v>15</v>
@@ -1576,11 +1977,8 @@
       <c r="N1" t="s">
         <v>77</v>
       </c>
-      <c r="O1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1620,11 +2018,8 @@
       <c r="M2">
         <v>0</v>
       </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1667,11 +2062,8 @@
       <c r="N3" t="s">
         <v>75</v>
       </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1714,11 +2106,8 @@
       <c r="N4" t="s">
         <v>75</v>
       </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1761,11 +2150,8 @@
       <c r="N5" t="s">
         <v>75</v>
       </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1808,11 +2194,8 @@
       <c r="N6" t="s">
         <v>75</v>
       </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1855,11 +2238,8 @@
       <c r="N7" t="s">
         <v>75</v>
       </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1902,11 +2282,8 @@
       <c r="N8" t="s">
         <v>75</v>
       </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1949,11 +2326,8 @@
       <c r="N9" t="s">
         <v>75</v>
       </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1993,11 +2367,8 @@
       <c r="M10">
         <v>0</v>
       </c>
-      <c r="O10">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2040,11 +2411,8 @@
       <c r="N11" t="s">
         <v>76</v>
       </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2087,11 +2455,8 @@
       <c r="N12" t="s">
         <v>76</v>
       </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2134,16 +2499,13 @@
       <c r="N13" t="s">
         <v>76</v>
       </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -2158,7 +2520,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -2178,11 +2540,8 @@
       <c r="M14" s="1">
         <v>0</v>
       </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2193,10 +2552,10 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="E15">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -2222,11 +2581,8 @@
       <c r="M15">
         <v>0</v>
       </c>
-      <c r="O15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>13</v>
       </c>
@@ -2246,7 +2602,7 @@
         <v>0</v>
       </c>
       <c r="G16">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -2264,9 +2620,6 @@
         <v>10000</v>
       </c>
       <c r="M16" s="1">
-        <v>0</v>
-      </c>
-      <c r="O16">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Model changes for explicit energy assets (via default energy assets)
*Model changes for explicit energy assets (via default energy assets)
*default assets have been added to option lists and databases.
</commit_message>
<xml_diff>
--- a/Base/db_defaultEnergyAssets.xlsx
+++ b/Base/db_defaultEnergyAssets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737D6D19-C2F8-42DE-9A9E-62C0A5AD2A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B9FA77-4747-432D-B056-49F2A6D517DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
   </bookViews>
   <sheets>
     <sheet name="consumptionAssets" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="130">
   <si>
     <t>id</t>
   </si>
@@ -406,19 +406,28 @@
     <t>Solarpanels_5MW</t>
   </si>
   <si>
-    <t>Solarpanels_6MW</t>
-  </si>
-  <si>
     <t>Solar field 5 MW</t>
   </si>
   <si>
-    <t>Solar field 6 MW</t>
-  </si>
-  <si>
     <t>Solar field 0 MW</t>
   </si>
   <si>
     <t>Building_heatpump_20kW</t>
+  </si>
+  <si>
+    <t>energy_consumption_kwhpkm</t>
+  </si>
+  <si>
+    <t>Solar panels for building, 10 kWp</t>
+  </si>
+  <si>
+    <t>Solarpanels_10MW</t>
+  </si>
+  <si>
+    <t>Solar field 10 MW</t>
+  </si>
+  <si>
+    <t>Building_solarpanels_10kWp</t>
   </si>
 </sst>
 </file>
@@ -778,7 +787,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1034,10 +1043,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E4F107-16BA-4AA1-967F-7283CFA19530}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1221,7 +1230,7 @@
         <v>106</v>
       </c>
       <c r="C8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
@@ -1324,6 +1333,9 @@
       <c r="F12">
         <v>4000</v>
       </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -1333,7 +1345,7 @@
         <v>121</v>
       </c>
       <c r="C13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
@@ -1343,6 +1355,9 @@
       </c>
       <c r="F13">
         <v>5000</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1350,10 +1365,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C14" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D14" t="s">
         <v>8</v>
@@ -1363,6 +1378,9 @@
       </c>
       <c r="F14">
         <v>6000</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1500,6 +1518,29 @@
         <v>5</v>
       </c>
       <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>129</v>
+      </c>
+      <c r="C21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21">
+        <v>10</v>
+      </c>
+      <c r="G21">
         <v>0</v>
       </c>
     </row>
@@ -1512,8 +1553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE703926-9782-410D-9F5D-95B93C05724F}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1522,6 +1563,7 @@
     <col min="3" max="3" width="24.1640625" customWidth="1"/>
     <col min="4" max="5" width="21.6640625" customWidth="1"/>
     <col min="6" max="6" width="17.1640625" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -1885,7 +1927,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -1916,10 +1958,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AD685B-9C82-478E-8117-8BE8411F8B92}">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1934,7 +1976,7 @@
     <col min="14" max="14" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1977,8 +2019,11 @@
       <c r="N1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2018,8 +2063,11 @@
       <c r="M2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2062,8 +2110,11 @@
       <c r="N3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2106,8 +2157,11 @@
       <c r="N4" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2150,8 +2204,11 @@
       <c r="N5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2194,8 +2251,11 @@
       <c r="N6" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2238,8 +2298,11 @@
       <c r="N7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2282,8 +2345,11 @@
       <c r="N8" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2326,8 +2392,11 @@
       <c r="N9" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2367,8 +2436,11 @@
       <c r="M10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2411,8 +2483,11 @@
       <c r="N11" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2455,8 +2530,11 @@
       <c r="N12" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2499,8 +2577,11 @@
       <c r="N13" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2540,8 +2621,11 @@
       <c r="M14" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2581,8 +2665,11 @@
       <c r="M15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O15">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>13</v>
       </c>
@@ -2620,6 +2707,9 @@
         <v>10000</v>
       </c>
       <c r="M16" s="1">
+        <v>0</v>
+      </c>
+      <c r="O16">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EV and EHGV hourly load profiles calculated and exported
*EV and EHGV total load profiles worden elke tijdstap opgehaald en aan het einde van de modelrun geëxporteerd met de totalCostKPI's
*gemiddelde netto load van alle voertuigen van het type EV, EHGV (trucks). Teruglevering = negatieve load.
</commit_message>
<xml_diff>
--- a/Base/db_defaultEnergyAssets.xlsx
+++ b/Base/db_defaultEnergyAssets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B9FA77-4747-432D-B056-49F2A6D517DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB74DB9-A2CC-4441-802D-285B9DAD342B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
   </bookViews>
   <sheets>
     <sheet name="consumptionAssets" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="129">
   <si>
     <t>id</t>
   </si>
@@ -323,9 +323,6 @@
   </si>
   <si>
     <t>EHGV</t>
-  </si>
-  <si>
-    <t>ELECTRIC_HEAVY_GOODS_VEHICLE</t>
   </si>
   <si>
     <t>storageCapacity_kWh</t>
@@ -1017,10 +1014,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" t="s">
         <v>97</v>
-      </c>
-      <c r="C10" t="s">
-        <v>98</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
@@ -1045,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E4F107-16BA-4AA1-967F-7283CFA19530}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1227,10 +1224,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
@@ -1273,10 +1270,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
@@ -1296,10 +1293,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
@@ -1319,10 +1316,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
@@ -1342,10 +1339,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C13" t="s">
         <v>121</v>
-      </c>
-      <c r="C13" t="s">
-        <v>122</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
@@ -1365,10 +1362,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" t="s">
         <v>127</v>
-      </c>
-      <c r="C14" t="s">
-        <v>128</v>
       </c>
       <c r="D14" t="s">
         <v>8</v>
@@ -1388,10 +1385,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" t="s">
         <v>103</v>
-      </c>
-      <c r="C15" t="s">
-        <v>104</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
@@ -1411,10 +1408,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" t="s">
         <v>101</v>
-      </c>
-      <c r="C16" t="s">
-        <v>102</v>
       </c>
       <c r="D16" t="s">
         <v>8</v>
@@ -1434,10 +1431,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D17" t="s">
         <v>8</v>
@@ -1457,10 +1454,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D18" t="s">
         <v>8</v>
@@ -1480,10 +1477,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D19" t="s">
         <v>8</v>
@@ -1503,10 +1500,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D20" t="s">
         <v>8</v>
@@ -1526,10 +1523,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D21" t="s">
         <v>8</v>
@@ -1901,7 +1898,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -1927,7 +1924,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -1960,8 +1957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AD685B-9C82-478E-8117-8BE8411F8B92}">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2011,7 +2008,7 @@
         <v>12</v>
       </c>
       <c r="L1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M1" t="s">
         <v>15</v>
@@ -2020,7 +2017,7 @@
         <v>77</v>
       </c>
       <c r="O1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -2586,7 +2583,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -2636,10 +2633,10 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>95</v>
+        <v>20</v>
       </c>
       <c r="E15">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -2666,7 +2663,7 @@
         <v>0</v>
       </c>
       <c r="O15">
-        <v>0.4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -2674,7 +2671,7 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
DieselTrucks and total system Diesel Import MWh KPI
*DieselVehicles are made possible, with which trucks are modeled, both as individual trucks and as scaled single vehicle.
*Total system Diesel Import MWh KPI is added to totalCostKPI's output json, useful for CO2 and energy carrier costs calculations
</commit_message>
<xml_diff>
--- a/Base/db_defaultEnergyAssets.xlsx
+++ b/Base/db_defaultEnergyAssets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4FC580-FF5B-4807-8DBC-390D35C00ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105E1021-EF08-45FA-887B-B1B8BD9187A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
   </bookViews>
   <sheets>
     <sheet name="consumptionAssets" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="133">
   <si>
     <t>id</t>
   </si>
@@ -433,10 +433,10 @@
     <t>vehicle_scaling</t>
   </si>
   <si>
-    <t>TruckDiesel</t>
-  </si>
-  <si>
-    <t>VEHICLE</t>
+    <t>DieselTruck</t>
+  </si>
+  <si>
+    <t>DIESEL_VEHICLE</t>
   </si>
 </sst>
 </file>
@@ -1560,10 +1560,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE703926-9782-410D-9F5D-95B93C05724F}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1575,7 +1575,7 @@
     <col min="8" max="8" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1603,8 +1603,14 @@
       <c r="I1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>124</v>
+      </c>
+      <c r="K1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1633,7 +1639,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1662,7 +1668,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1691,7 +1697,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1717,7 +1723,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1746,7 +1752,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1772,7 +1778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1798,7 +1804,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1827,7 +1833,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1853,7 +1859,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1879,7 +1885,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1905,7 +1911,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1931,7 +1937,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1960,7 +1966,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1972,6 +1978,21 @@
       </c>
       <c r="D15" t="s">
         <v>132</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0.2</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1983,8 +2004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AD685B-9C82-478E-8117-8BE8411F8B92}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
No more default assets
Config is now the only way to add energy assets.
Also for households and industry
</commit_message>
<xml_diff>
--- a/Base/db_defaultEnergyAssets.xlsx
+++ b/Base/db_defaultEnergyAssets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20180652\OneDrive - TU Eindhoven\Documents\GitHub\Holon\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105E1021-EF08-45FA-887B-B1B8BD9187A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0772EB9E-B43C-4B3C-85F4-95A39E0AC095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CA7A310D-0CA1-49A6-840A-55868387A1DA}"/>
   </bookViews>
   <sheets>
     <sheet name="consumptionAssets" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -106,9 +105,6 @@
     <t>alias</t>
   </si>
   <si>
-    <t>OTHER_ELECTRICITY_CONSUMPTION</t>
-  </si>
-  <si>
     <t>HOT_WATER_CONSUMPTION</t>
   </si>
   <si>
@@ -437,6 +433,9 @@
   </si>
   <si>
     <t>DIESEL_VEHICLE</t>
+  </si>
+  <si>
+    <t>ELECTRICITY_CONSUMPTION_PROFILE</t>
   </si>
 </sst>
 </file>
@@ -796,7 +795,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -829,10 +828,10 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
         <v>63</v>
-      </c>
-      <c r="G1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -840,16 +839,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>132</v>
       </c>
       <c r="F2">
         <v>2479</v>
@@ -863,16 +862,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -886,16 +885,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>132</v>
       </c>
       <c r="F4">
         <f>60*2000</f>
@@ -910,16 +909,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>132</v>
       </c>
       <c r="F5">
         <f>35*1000</f>
@@ -934,16 +933,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F6">
         <v>1000000</v>
@@ -957,16 +956,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -980,16 +979,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F8">
         <v>1000000</v>
@@ -1003,16 +1002,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1026,16 +1025,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" t="s">
         <v>96</v>
-      </c>
-      <c r="C10" t="s">
-        <v>97</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F10">
         <f>50*100000*1.3</f>
@@ -1094,10 +1093,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -1118,10 +1117,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -1142,10 +1141,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
@@ -1166,16 +1165,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5">
         <f>3000</f>
@@ -1190,16 +1189,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6">
         <v>5000</v>
@@ -1213,16 +1212,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7">
         <v>7000</v>
@@ -1236,10 +1235,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
@@ -1259,10 +1258,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
@@ -1282,10 +1281,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
@@ -1305,10 +1304,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
@@ -1328,10 +1327,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
@@ -1351,10 +1350,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" t="s">
         <v>120</v>
-      </c>
-      <c r="C13" t="s">
-        <v>121</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
@@ -1374,10 +1373,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" t="s">
         <v>126</v>
-      </c>
-      <c r="C14" t="s">
-        <v>127</v>
       </c>
       <c r="D14" t="s">
         <v>8</v>
@@ -1397,10 +1396,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" t="s">
         <v>102</v>
-      </c>
-      <c r="C15" t="s">
-        <v>103</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
@@ -1420,10 +1419,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" t="s">
         <v>100</v>
-      </c>
-      <c r="C16" t="s">
-        <v>101</v>
       </c>
       <c r="D16" t="s">
         <v>8</v>
@@ -1443,10 +1442,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D17" t="s">
         <v>8</v>
@@ -1466,10 +1465,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D18" t="s">
         <v>8</v>
@@ -1489,10 +1488,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D19" t="s">
         <v>8</v>
@@ -1512,10 +1511,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D20" t="s">
         <v>8</v>
@@ -1535,10 +1534,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D21" t="s">
         <v>8</v>
@@ -1562,7 +1561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE703926-9782-410D-9F5D-95B93C05724F}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
@@ -1598,16 +1597,16 @@
         <v>18</v>
       </c>
       <c r="H1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1615,13 +1614,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2">
         <v>4</v>
@@ -1636,7 +1635,7 @@
         <v>60</v>
       </c>
       <c r="I2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -1644,13 +1643,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3">
         <v>6</v>
@@ -1665,7 +1664,7 @@
         <v>60</v>
       </c>
       <c r="I3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -1673,13 +1672,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4">
         <v>11</v>
@@ -1694,7 +1693,7 @@
         <v>60</v>
       </c>
       <c r="I4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -1702,13 +1701,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1728,13 +1727,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1749,7 +1748,7 @@
         <v>90</v>
       </c>
       <c r="I6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -1783,13 +1782,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1809,13 +1808,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -1830,7 +1829,7 @@
         <v>90</v>
       </c>
       <c r="I9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -1838,13 +1837,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E10">
         <v>300</v>
@@ -1864,13 +1863,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1890,13 +1889,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1916,13 +1915,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1942,13 +1941,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E14">
         <v>20</v>
@@ -1963,7 +1962,7 @@
         <v>60</v>
       </c>
       <c r="I14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -1971,13 +1970,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -2004,8 +2003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AD685B-9C82-478E-8117-8BE8411F8B92}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2049,25 +2048,25 @@
         <v>14</v>
       </c>
       <c r="J1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K1" t="s">
         <v>12</v>
       </c>
       <c r="L1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M1" t="s">
         <v>15</v>
       </c>
       <c r="N1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -2075,13 +2074,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -2111,6 +2110,9 @@
         <v>0</v>
       </c>
       <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
         <v>0</v>
       </c>
     </row>
@@ -2119,13 +2121,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -2155,9 +2157,12 @@
         <v>10000000</v>
       </c>
       <c r="N3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
         <v>0</v>
       </c>
     </row>
@@ -2166,13 +2171,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -2202,9 +2207,12 @@
         <v>10000000</v>
       </c>
       <c r="N4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
         <v>0</v>
       </c>
     </row>
@@ -2213,13 +2221,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -2249,9 +2257,12 @@
         <v>10000000</v>
       </c>
       <c r="N5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
         <v>0</v>
       </c>
     </row>
@@ -2260,13 +2271,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -2296,9 +2307,12 @@
         <v>10000000</v>
       </c>
       <c r="N6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
         <v>0</v>
       </c>
     </row>
@@ -2307,13 +2321,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -2343,9 +2357,12 @@
         <v>10000000</v>
       </c>
       <c r="N7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
         <v>0</v>
       </c>
     </row>
@@ -2354,13 +2371,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -2390,9 +2407,12 @@
         <v>10000000</v>
       </c>
       <c r="N8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
         <v>0</v>
       </c>
     </row>
@@ -2401,13 +2421,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -2437,9 +2457,12 @@
         <v>10000000</v>
       </c>
       <c r="N9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
         <v>0</v>
       </c>
     </row>
@@ -2486,19 +2509,22 @@
       <c r="O10">
         <v>0.2</v>
       </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -2528,9 +2554,12 @@
         <v>10000000000</v>
       </c>
       <c r="N11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
         <v>0</v>
       </c>
     </row>
@@ -2539,13 +2568,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -2575,9 +2604,12 @@
         <v>10000000</v>
       </c>
       <c r="N12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
         <v>0</v>
       </c>
     </row>
@@ -2586,13 +2618,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -2622,9 +2654,12 @@
         <v>10000000</v>
       </c>
       <c r="N13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
         <v>0</v>
       </c>
     </row>
@@ -2633,13 +2668,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14">
         <v>1000</v>
@@ -2669,6 +2704,9 @@
         <v>0</v>
       </c>
       <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
         <v>0</v>
       </c>
     </row>
@@ -2677,7 +2715,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -2713,6 +2751,9 @@
         <v>0</v>
       </c>
       <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
         <v>1</v>
       </c>
     </row>
@@ -2721,13 +2762,13 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E16">
         <v>2000</v>
@@ -2757,6 +2798,9 @@
         <v>0</v>
       </c>
       <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
         <v>0</v>
       </c>
     </row>
@@ -2765,13 +2809,13 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E17">
         <v>50</v>

</xml_diff>